<commit_message>
feat: pay tickect callback && add excel extend
</commit_message>
<xml_diff>
--- a/battleworld/Excel/PropDrop_可拾取物.xlsx
+++ b/battleworld/Excel/PropDrop_可拾取物.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15800" windowWidth="28040" xWindow="4240" yWindow="640"/>
+    <workbookView windowHeight="17655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcMode="auto"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,53 +27,561 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve">  </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Discribe</t>
+  </si>
+  <si>
+    <t>dropType</t>
+  </si>
+  <si>
+    <t>dropGuid</t>
+  </si>
+  <si>
+    <t>rewardFly</t>
+  </si>
+  <si>
+    <t>upTime</t>
+  </si>
+  <si>
+    <t>rewardMove</t>
+  </si>
+  <si>
+    <t>rewardOffsetZ</t>
+  </si>
+  <si>
+    <t>fallTime</t>
+  </si>
+  <si>
+    <t>overTime</t>
+  </si>
+  <si>
+    <t>extend</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>1技能 2血瓶 3金币 4丹药 5化形丹</t>
+  </si>
+  <si>
+    <t>掉落预制体guid</t>
+  </si>
+  <si>
+    <t>奖励飞行最大高度相对</t>
+  </si>
+  <si>
+    <t>上升时间秒</t>
+  </si>
+  <si>
+    <t>奖励移动最大距离相对</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奖励落地相对高度相对
+</t>
+  </si>
+  <si>
+    <t>下落时间</t>
+  </si>
+  <si>
+    <t>掉落物销毁时间(0代表不消失 秒)</t>
+  </si>
+  <si>
+    <t>扩展字段(用来存属性值)</t>
+  </si>
+  <si>
+    <t>金币</t>
+  </si>
+  <si>
+    <t>5BA0F2F74122E218BA6564B648CF5704</t>
+  </si>
+  <si>
+    <t>{"value":100}</t>
+  </si>
+  <si>
+    <t>技能球</t>
+  </si>
+  <si>
+    <t>147DCB9A4B7FDB75926F50B33104E415</t>
+  </si>
+  <si>
+    <t>血瓶</t>
+  </si>
+  <si>
+    <t>7AB4F8694A94CEFB2FA21989A0E3E3D2</t>
+  </si>
+  <si>
+    <t>{"value":10}</t>
+  </si>
+  <si>
+    <t>化形丹</t>
+  </si>
+  <si>
+    <t>888F269A495A38DFBB5D94BF9F5BEBE2</t>
+  </si>
+  <si>
+    <t>初阶-养气丹</t>
+  </si>
+  <si>
+    <t>9C82E15B4D7AC08F2AE87690A4A738A5</t>
+  </si>
+  <si>
+    <t>{"attributeID":107,"attributeValue":100,"duration":150}</t>
+  </si>
+  <si>
+    <t>初阶-生骨丹</t>
+  </si>
+  <si>
+    <t>77B3466B4299EEB7FAB627A6E8B7AA5E</t>
+  </si>
+  <si>
+    <t>{"attributeID":102,"attributeValue":100,"duration":150}</t>
+  </si>
+  <si>
+    <t>初阶-龙鳞丹</t>
+  </si>
+  <si>
+    <t>986105E84C483273F2A5E09ACDF2FA41</t>
+  </si>
+  <si>
+    <t>{"attributeID":104,"attributeValue":10,"duration":150}</t>
+  </si>
+  <si>
+    <t>初阶-龟甲丹</t>
+  </si>
+  <si>
+    <t>A97431DE41AFDD8113C9B4BE2245036F</t>
+  </si>
+  <si>
+    <t>{"attributeID":203,"attributeValue":5,"duration":150}</t>
+  </si>
+  <si>
+    <t>化形丹·鸣人</t>
+  </si>
+  <si>
+    <t>54E92DF14E6C1AA4550A80BFDD63666F</t>
+  </si>
+  <si>
+    <t>化形丹·路飞</t>
+  </si>
+  <si>
+    <t>86C7FA9D431FF7D2A1D539BD96154B22</t>
+  </si>
+  <si>
+    <t>化形丹·蛋仔</t>
+  </si>
+  <si>
+    <t>501DEBDD4B19EBAE54DF18BB6D31CEAA</t>
+  </si>
+  <si>
+    <t>化形丹·索隆</t>
+  </si>
+  <si>
+    <t>C25762B8499159FBFE32B2BE7E5B4E7D</t>
+  </si>
+  <si>
+    <t>化形丹·樱校女</t>
+  </si>
+  <si>
+    <t>29C967E94618A6CA4D8F1899A4F80C3A</t>
+  </si>
+  <si>
+    <t>化形丹·卡卡西</t>
+  </si>
+  <si>
+    <t>1EA5D94C4B050095070661BBDD6F38D0</t>
+  </si>
+  <si>
+    <t>化形丹·樱校男</t>
+  </si>
+  <si>
+    <t>341EEB6A41FA27832FA1E6B84090417C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9.75"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9.75"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125">
-        <fgColor/>
-        <bgColor/>
+  <fills count="33">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -80,45 +590,317 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -167,7 +949,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -200,26 +982,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -252,23 +1017,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -410,148 +1158,137 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3 xr6 xr10 x15">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
-    <outlinePr summaryBelow="false" summaryRight="false"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView showGridLines="true" tabSelected="true" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="19"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="4" min="4" style="0" width="55"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="7" min="7" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="8" min="8" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="9" min="9" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="10" min="10" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="11" min="11" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="12" min="12" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="13" min="13" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="14" min="14" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="15" min="15" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="16" min="16" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="17" min="17" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="18" min="18" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="19" min="19" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="20" min="20" style="0" width="15"/>
+    <col min="1" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="55" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="20" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="true" ht="21" r="1">
-      <c r="A1" s="1" t="str">
-        <v>int</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <v>string</v>
-      </c>
-      <c r="C1" s="1" t="str">
-        <v>int</v>
-      </c>
-      <c r="D1" s="1" t="str">
-        <v>string</v>
-      </c>
-      <c r="E1" s="1" t="str">
-        <v>int</v>
-      </c>
-      <c r="F1" s="1" t="str">
-        <v>float</v>
-      </c>
-      <c r="G1" s="1" t="str">
-        <v>int</v>
-      </c>
-      <c r="H1" s="1" t="str">
-        <v>int</v>
-      </c>
-      <c r="I1" s="1" t="str">
-        <v>float</v>
-      </c>
-      <c r="J1" s="1" t="str">
-        <v>float</v>
+    <row r="1" ht="21" customHeight="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="2">
-      <c r="A2" s="1" t="str">
-        <v>id</v>
-      </c>
-      <c r="B2" s="1" t="str">
-        <v>Discribe</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <v>dropType</v>
-      </c>
-      <c r="D2" s="1" t="str">
-        <v>dropGuid</v>
-      </c>
-      <c r="E2" s="1" t="str">
-        <v>rewardFly</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <v>upTime</v>
-      </c>
-      <c r="G2" s="1" t="str">
-        <v>rewardMove</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <v>rewardOffsetZ</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <v>fallTime</v>
-      </c>
-      <c r="J2" s="1" t="str">
-        <v>overTime</v>
+    <row r="2" ht="21" customHeight="1" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="3">
-      <c r="A3" s="1" t="str">
-        <v>id</v>
-      </c>
-      <c r="B3" s="1" t="str">
-        <v>描述</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <v>1技能 2血瓶 3金币 4丹药 5化形丹</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <v>掉落预制体guid</v>
-      </c>
-      <c r="E3" s="1" t="str">
-        <v>奖励飞行最大高度相对</v>
-      </c>
-      <c r="F3" s="1" t="str">
-        <v>上升时间秒</v>
-      </c>
-      <c r="G3" s="1" t="str">
-        <v>奖励移动最大距离相对</v>
-      </c>
-      <c r="H3" s="1" t="str">
-        <v>奖励落地相对高度相对
-</v>
-      </c>
-      <c r="I3" s="1" t="str">
-        <v>下落时间</v>
-      </c>
-      <c r="J3" s="1" t="str">
-        <v>掉落物销毁时间(0代表不消失 秒)</v>
+    <row r="3" ht="21" customHeight="1" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="4">
+    <row r="4" ht="21" customHeight="1" spans="1:10">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -563,18 +1300,18 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row customHeight="true" ht="21" r="5">
+    <row r="5" ht="21" customHeight="1" spans="1:11">
       <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="str">
-        <v>金币</v>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="str">
-        <v>5BA0F2F74122E218BA6564B648CF5704</v>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="E5" s="1">
         <v>200</v>
@@ -594,19 +1331,22 @@
       <c r="J5" s="1">
         <v>10</v>
       </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row customHeight="true" ht="21" r="6">
+    <row r="6" ht="21" customHeight="1" spans="1:10">
       <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="str">
-        <v>技能球</v>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <v>147DCB9A4B7FDB75926F50B33104E415</v>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="E6" s="1">
         <v>200</v>
@@ -627,18 +1367,18 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="7">
+    <row r="7" ht="21" customHeight="1" spans="1:11">
       <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="str">
-        <v>血瓶</v>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="str">
-        <v>7AB4F8694A94CEFB2FA21989A0E3E3D2</v>
+      <c r="D7" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>200</v>
@@ -658,19 +1398,22 @@
       <c r="J7" s="1">
         <v>10</v>
       </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row customHeight="true" ht="21" r="8">
+    <row r="8" ht="21" customHeight="1" spans="1:10">
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="str">
-        <v>化形丹</v>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="D8" s="1" t="str">
-        <v>888F269A495A38DFBB5D94BF9F5BEBE2</v>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E8" s="1">
         <v>200</v>
@@ -691,18 +1434,18 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="9">
+    <row r="9" ht="21" customHeight="1" spans="1:11">
       <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="str">
-        <v>初阶-养气丹</v>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C9" s="1">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="str">
-        <v>9C82E15B4D7AC08F2AE87690A4A738A5</v>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E9" s="1">
         <v>200</v>
@@ -722,19 +1465,22 @@
       <c r="J9" s="1">
         <v>10</v>
       </c>
+      <c r="K9" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row customHeight="true" ht="21" r="10">
+    <row r="10" ht="21" customHeight="1" spans="1:11">
       <c r="A10" s="1">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="str">
-        <v>初阶-生骨丹</v>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="1">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="str">
-        <v>77B3466B4299EEB7FAB627A6E8B7AA5E</v>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E10" s="1">
         <v>200</v>
@@ -754,19 +1500,22 @@
       <c r="J10" s="1">
         <v>10</v>
       </c>
+      <c r="K10" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row customHeight="true" ht="21" r="11">
+    <row r="11" ht="21" customHeight="1" spans="1:11">
       <c r="A11" s="1">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="str">
-        <v>初阶-龙鳞丹</v>
+      <c r="B11" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C11" s="1">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="str">
-        <v>986105E84C483273F2A5E09ACDF2FA41</v>
+      <c r="D11" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E11" s="1">
         <v>200</v>
@@ -786,19 +1535,22 @@
       <c r="J11" s="1">
         <v>10</v>
       </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row customHeight="true" ht="21" r="12">
+    <row r="12" ht="21" customHeight="1" spans="1:11">
       <c r="A12" s="1">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="str">
-        <v>初阶-龟甲丹</v>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="C12" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="1" t="str">
-        <v>A97431DE41AFDD8113C9B4BE2245036F</v>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="E12" s="1">
         <v>200</v>
@@ -818,19 +1570,22 @@
       <c r="J12" s="1">
         <v>10</v>
       </c>
+      <c r="K12" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row customHeight="true" ht="21" r="13">
+    <row r="13" ht="21" customHeight="1" spans="1:10">
       <c r="A13" s="1">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="str">
-        <v>化形丹·鸣人</v>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C13" s="1">
         <v>5</v>
       </c>
-      <c r="D13" t="str">
-        <v>54E92DF14E6C1AA4550A80BFDD63666F</v>
+      <c r="D13" t="s">
+        <v>47</v>
       </c>
       <c r="E13" s="1">
         <v>200</v>
@@ -851,18 +1606,18 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="14">
+    <row r="14" ht="21" customHeight="1" spans="1:10">
       <c r="A14" s="1">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="str">
-        <v>化形丹·路飞</v>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C14" s="1">
         <v>5</v>
       </c>
-      <c r="D14" t="str">
-        <v>86C7FA9D431FF7D2A1D539BD96154B22</v>
+      <c r="D14" t="s">
+        <v>49</v>
       </c>
       <c r="E14" s="1">
         <v>200</v>
@@ -883,18 +1638,18 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="15">
+    <row r="15" ht="21" customHeight="1" spans="1:10">
       <c r="A15" s="1">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="str">
-        <v>化形丹·蛋仔</v>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C15" s="1">
         <v>5</v>
       </c>
-      <c r="D15" t="str">
-        <v>501DEBDD4B19EBAE54DF18BB6D31CEAA</v>
+      <c r="D15" t="s">
+        <v>51</v>
       </c>
       <c r="E15" s="1">
         <v>200</v>
@@ -915,18 +1670,18 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="16">
+    <row r="16" ht="21" customHeight="1" spans="1:10">
       <c r="A16" s="1">
         <v>12</v>
       </c>
-      <c r="B16" s="2" t="str">
-        <v>化形丹·索隆</v>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
       </c>
-      <c r="D16" t="str">
-        <v>C25762B8499159FBFE32B2BE7E5B4E7D</v>
+      <c r="D16" t="s">
+        <v>53</v>
       </c>
       <c r="E16" s="1">
         <v>200</v>
@@ -947,18 +1702,18 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="17">
+    <row r="17" ht="21" customHeight="1" spans="1:10">
       <c r="A17" s="1">
         <v>13</v>
       </c>
-      <c r="B17" s="2" t="str">
-        <v>化形丹·樱校女</v>
+      <c r="B17" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C17" s="1">
         <v>5</v>
       </c>
-      <c r="D17" t="str">
-        <v>29C967E94618A6CA4D8F1899A4F80C3A</v>
+      <c r="D17" t="s">
+        <v>55</v>
       </c>
       <c r="E17" s="1">
         <v>200</v>
@@ -979,18 +1734,18 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="18">
+    <row r="18" ht="21" customHeight="1" spans="1:10">
       <c r="A18" s="1">
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="str">
-        <v>化形丹·卡卡西</v>
+      <c r="B18" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
       </c>
-      <c r="D18" t="str">
-        <v>1EA5D94C4B050095070661BBDD6F38D0</v>
+      <c r="D18" t="s">
+        <v>57</v>
       </c>
       <c r="E18" s="1">
         <v>200</v>
@@ -1011,18 +1766,18 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="19">
-      <c r="A19" s="2">
+    <row r="19" ht="21" customHeight="1" spans="1:10">
+      <c r="A19" s="1">
         <v>15</v>
       </c>
-      <c r="B19" s="2" t="str">
-        <v>化形丹·樱校男</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="1">
         <v>5</v>
       </c>
-      <c r="D19" t="str">
-        <v>341EEB6A41FA27832FA1E6B84090417C</v>
+      <c r="D19" t="s">
+        <v>59</v>
       </c>
       <c r="E19" s="1">
         <v>200</v>
@@ -1043,9 +1798,10 @@
         <v>10</v>
       </c>
     </row>
-    <row customHeight="true" ht="21" r="20"/>
+    <row r="20" ht="21" customHeight="1"/>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <picture r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add pickup validate
</commit_message>
<xml_diff>
--- a/battleworld/Excel/PropDrop_可拾取物.xlsx
+++ b/battleworld/Excel/PropDrop_可拾取物.xlsx
@@ -68,7 +68,7 @@
     <t>overTime</t>
   </si>
   <si>
-    <t>extend</t>
+    <t>extends</t>
   </si>
   <si>
     <t>描述</t>
@@ -1169,7 +1169,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75"/>

</xml_diff>